<commit_message>
[FIX] knn clasificator fix format and dectet that data was not being used only random data which affected accuracy tremendusly
</commit_message>
<xml_diff>
--- a/data/properties.xlsx
+++ b/data/properties.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Documentos\u\11.Semester_XI\TIA\Computer-Vision\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4366BAE-D3FB-4111-A1E9-5E4FD7F6EAB8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BD485E1-09B0-4A20-9138-FC072A976048}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="7140" yWindow="0" windowWidth="11520" windowHeight="12360" xr2:uid="{7211C498-63A5-494B-97AD-585ED88DF649}"/>
   </bookViews>
@@ -1386,8 +1386,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FF51B139-E601-4365-8BB4-713603159F5C}">
   <dimension ref="A1:Q677"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B626" workbookViewId="0">
-      <selection activeCell="C629" sqref="C629"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -33590,7 +33590,7 @@
         <v>269</v>
       </c>
       <c r="C608" s="1" t="s">
-        <v>254</v>
+        <v>308</v>
       </c>
       <c r="D608">
         <v>2.1599478336472972E+16</v>
@@ -34756,7 +34756,7 @@
         <v>278</v>
       </c>
       <c r="C630" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D630">
         <v>2.1414225654462244E+16</v>
@@ -34809,7 +34809,7 @@
         <v>280</v>
       </c>
       <c r="C631" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D631">
         <v>3.0926913423065552E+16</v>
@@ -34915,7 +34915,7 @@
         <v>280</v>
       </c>
       <c r="C633" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D633">
         <v>224062294615198</v>
@@ -34968,7 +34968,7 @@
         <v>281</v>
       </c>
       <c r="C634" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D634">
         <v>2.1539940930008928E+16</v>
@@ -35021,7 +35021,7 @@
         <v>282</v>
       </c>
       <c r="C635" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D635">
         <v>2.1684825027161384E+16</v>
@@ -35074,7 +35074,7 @@
         <v>282</v>
       </c>
       <c r="C636" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D636">
         <v>2.1365649723822712E+16</v>
@@ -35127,7 +35127,7 @@
         <v>283</v>
       </c>
       <c r="C637" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D637">
         <v>1378503012672156</v>
@@ -35233,7 +35233,7 @@
         <v>285</v>
       </c>
       <c r="C639" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D639">
         <v>2.2399275285122492E+16</v>
@@ -35339,7 +35339,7 @@
         <v>286</v>
       </c>
       <c r="C641" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D641">
         <v>2.1980259633925036E+16</v>
@@ -35392,7 +35392,7 @@
         <v>287</v>
       </c>
       <c r="C642" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D642">
         <v>2.3555583157952808E+16</v>
@@ -35498,7 +35498,7 @@
         <v>288</v>
       </c>
       <c r="C644" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D644">
         <v>1392174993227894</v>
@@ -35551,7 +35551,7 @@
         <v>288</v>
       </c>
       <c r="C645" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D645">
         <v>2147895463999566</v>
@@ -35604,7 +35604,7 @@
         <v>289</v>
       </c>
       <c r="C646" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D646">
         <v>2.3162647172822928E+16</v>
@@ -35657,7 +35657,7 @@
         <v>290</v>
       </c>
       <c r="C647" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D647">
         <v>229782149930756</v>
@@ -35763,7 +35763,7 @@
         <v>292</v>
       </c>
       <c r="C649" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D649">
         <v>1.4635032291422784E+16</v>
@@ -35922,7 +35922,7 @@
         <v>294</v>
       </c>
       <c r="C652" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D652">
         <v>2.3712579216279876E+16</v>
@@ -36028,7 +36028,7 @@
         <v>296</v>
       </c>
       <c r="C654" s="1" t="s">
-        <v>279</v>
+        <v>308</v>
       </c>
       <c r="D654">
         <v>2.2678176455080872E+16</v>
@@ -36081,7 +36081,7 @@
         <v>297</v>
       </c>
       <c r="C655" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D655">
         <v>1.3728226761172266E+16</v>
@@ -36134,7 +36134,7 @@
         <v>297</v>
       </c>
       <c r="C656" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D656">
         <v>2.2771219815869912E+16</v>
@@ -36187,7 +36187,7 @@
         <v>297</v>
       </c>
       <c r="C657" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D657">
         <v>2.1143346202105192E+16</v>
@@ -36240,7 +36240,7 @@
         <v>297</v>
       </c>
       <c r="C658" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D658">
         <v>2.1762790209874792E+16</v>
@@ -36770,7 +36770,7 @@
         <v>304</v>
       </c>
       <c r="C668" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D668">
         <v>2.2967866777303208E+16</v>
@@ -36823,7 +36823,7 @@
         <v>304</v>
       </c>
       <c r="C669" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D669">
         <v>2.2735648930304344E+16</v>
@@ -36876,7 +36876,7 @@
         <v>304</v>
       </c>
       <c r="C670" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D670">
         <v>2.2732855546058256E+16</v>
@@ -36982,7 +36982,7 @@
         <v>305</v>
       </c>
       <c r="C672" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D672">
         <v>2.1030137503701996E+16</v>
@@ -37035,7 +37035,7 @@
         <v>305</v>
       </c>
       <c r="C673" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D673">
         <v>2.3252916201790748E+16</v>
@@ -37141,7 +37141,7 @@
         <v>306</v>
       </c>
       <c r="C675" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D675">
         <v>2.3251491940091448E+16</v>
@@ -37194,7 +37194,7 @@
         <v>306</v>
       </c>
       <c r="C676" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D676">
         <v>2110296944962923</v>
@@ -37247,7 +37247,7 @@
         <v>307</v>
       </c>
       <c r="C677" s="1" t="s">
-        <v>298</v>
+        <v>308</v>
       </c>
       <c r="D677">
         <v>2.2337877001861776E+16</v>

</xml_diff>